<commit_message>
se generan los xml de bscs
</commit_message>
<xml_diff>
--- a/rsc/projects.xlsx
+++ b/rsc/projects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763A6F0D-0086-4811-9760-D06BDDB9F5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69EE9E3-B28F-4ABC-A15C-0B0EEC0F40BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2355" windowWidth="21600" windowHeight="11505" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Projects</t>
   </si>
   <si>
-    <t>TestRuben1</t>
+    <t>testeObregon</t>
   </si>
   <si>
-    <t>TestRuben2</t>
-  </si>
-  <si>
-    <t>TestRuben3</t>
+    <t>AmxCoMovPosPlan090</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +462,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -474,9 +471,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>

</xml_diff>